<commit_message>
stanza 추가, threshold 0.7로 조정
</commit_message>
<xml_diff>
--- a/pa/output.xlsx
+++ b/pa/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,7 +555,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>‘蒹葭(三章章八句)’至‘國焉’ 正義曰：作蒹葭詩者, 刺襄公也.</t>
+          <t>‘蒹葭(三章章八句)’至‘國焉’ 正義曰：作蒹葭詩者, 刺襄公也. 襄公新得周地, 其民被周之德敎日久.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.7598408468707351</v>
+        <v>0.7496557274694617</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -573,7 +573,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>襄公新得周地, 其民被周之德敎日久.今襄公未能用周禮以敎之.</t>
+          <t>‘蒹葭(三章章八句)’至‘國焉’ 正義曰：作蒹葭詩者, 刺襄公也. 襄公新得周地, 其民被周之德敎日久.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.5263518149750573</v>
+        <v>0.390050507484113</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -601,7 +601,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>禮者, 為國之本, 未能用周禮, 將無以固其國焉, 故刺之也.</t>
+          <t>今襄公未能用周禮以敎之. 禮者, 為國之本, 未能用周禮, 將無以固其國焉, 故刺之也. 經三章, 皆言治國須禮之事.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.441024032717669</v>
+        <v>0.5639870928375226</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -629,7 +629,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -639,7 +639,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>經三章, 皆言治國須禮之事.</t>
+          <t>今襄公未能用周禮以敎之. 禮者, 為國之本, 未能用周禮, 將無以固其國焉, 故刺之也. 經三章, 皆言治國須禮之事.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.4636741604720288</v>
+        <v>0.4185028618934107</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -657,7 +657,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>‘蒹葭’至‘中央’ [正義曰]</t>
+          <t>‘蒹葭’至‘中央’ [正義曰]：毛以為“蒹葭之草, 蒼蒼然雖盛, 未堪家用, 必待白露凝戾為霜, 然後堅實中用, 歲事得成, 以興秦國之民雖衆, 而未順德敎, 必待周禮以敎之, 然後服從上命, 國乃得興. 今襄公未能用周禮, 其國未得興也, 由未能用周禮, 故未得人服也. 所謂維是得人之道, 乃遠在大水一邊, 大水, 喻禮樂, 言得人之道, 乃在禮樂之一邊.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1096,7 +1096,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.4915723691084867</v>
+        <v>0.4417830326450587</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1105,7 +1105,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>：毛以為“蒹葭之草, 蒼蒼然雖盛, 未堪家用, 必待白露凝戾為霜, 然後堅實中用, 歲事得成, 以興秦國之民雖衆, 而未順德敎, 必待周禮以敎之, 然後服從上命, 國乃得興.</t>
+          <t>‘蒹葭’至‘中央’ [正義曰]：毛以為“蒹葭之草, 蒼蒼然雖盛, 未堪家用, 必待白露凝戾為霜, 然後堅實中用, 歲事得成, 以興秦國之民雖衆, 而未順德敎, 必待周禮以敎之, 然後服從上命, 國乃得興. 今襄公未能用周禮, 其國未得興也, 由未能用周禮, 故未得人服也. 所謂維是得人之道, 乃遠在大水一邊, 大水, 喻禮樂, 言得人之道, 乃在禮樂之一邊.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1124,7 +1124,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.4374020313892926</v>
+        <v>0.41753517412263</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>今襄公未能用周禮, 其國未得興也, 由未能用周禮, 故未得人服也.</t>
+          <t>‘蒹葭’至‘中央’ [正義曰]：毛以為“蒹葭之草, 蒼蒼然雖盛, 未堪家用, 必待白露凝戾為霜, 然後堅實中用, 歲事得成, 以興秦國之民雖衆, 而未順德敎, 必待周禮以敎之, 然後服從上命, 國乃得興. 今襄公未能用周禮, 其國未得興也, 由未能用周禮, 故未得人服也. 所謂維是得人之道, 乃遠在大水一邊, 大水, 喻禮樂, 言得人之道, 乃在禮樂之一邊.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.4790428656819363</v>
+        <v>0.3597439069739088</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>所謂維是得人之道, 乃遠在大水一邊, 大水, 喻禮樂, 言得人之道, 乃在禮樂之一邊.旣以水喻禮樂, 禮樂之傍有得人之道, 因從水內求之.</t>
+          <t>旣以水喻禮樂, 禮樂之傍有得人之道, 因從水內求之. 若逆流遡洄而往從之, 則道險阻且長遠, 不可得至, 言逆禮以治國, 則無得人道, 終不可至. 若順流遡游而往從之, 則宛然在於水之中央, 言順禮治國, 則得人之道, 自來迎己, 正近在禮樂之內. 然則非禮, 必不得人, 得人, 必能固國, 君何以不求用周禮乎.”</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1180,7 +1180,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.3876056179367598</v>
+        <v>0.3810354642113402</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>若逆流遡洄而往從之, 則道險阻且長遠, 不可得至, 言逆禮以治國, 則無得人道, 終不可至.</t>
+          <t>旣以水喻禮樂, 禮樂之傍有得人之道, 因從水內求之. 若逆流遡洄而往從之, 則道險阻且長遠, 不可得至, 言逆禮以治國, 則無得人道, 終不可至. 若順流遡游而往從之, 則宛然在於水之中央, 言順禮治國, 則得人之道, 自來迎己, 正近在禮樂之內. 然則非禮, 必不得人, 得人, 必能固國, 君何以不求用周禮乎.”</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1208,7 +1208,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.2963935740976248</v>
+        <v>0.4890872211225044</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>若順流遡游而往從之, 則宛然在於水之中央, 言順禮治國, 則得人之道, 自來迎己, 正近在禮樂之內.然則非禮, 必不得人, 得人, 必能固國, 君何以不求用周禮乎.”</t>
+          <t>旣以水喻禮樂, 禮樂之傍有得人之道, 因從水內求之. 若逆流遡洄而往從之, 則道險阻且長遠, 不可得至, 言逆禮以治國, 則無得人道, 終不可至. 若順流遡游而往從之, 則宛然在於水之中央, 言順禮治國, 則得人之道, 自來迎己, 正近在禮樂之內. 然則非禮, 必不得人, 得人, 必能固國, 君何以不求用周禮乎.”</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1236,7 +1236,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.4174451318962261</v>
+        <v>0.4380292313083999</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>鄭以為“蒹葭在衆草之中 蒼蒼然彊盛, 雖似不可雕傷, 至白露凝戾為霜, 則成而為黃矣, 以興衆民之彊者, 不從襄公敎令, 雖似不可屈服, 若得周禮以敎, 則衆民自然服矣.</t>
+          <t>鄭以為“蒹葭在衆草之中 蒼蒼然彊盛, 雖似不可雕傷, 至白露凝戾為霜, 則成而為黃矣, 以興衆民之彊者, 不從襄公敎令, 雖似不可屈服, 若得周禮以敎, 則衆民自然服矣. 欲求周禮, 當得知周禮之人, 所謂是知周禮之人在於何處. 在大水之一邊, 假喻以言遠. 旣言此人在水一邊, 因以水行為喻.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1264,7 +1264,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.4805761182825232</v>
+        <v>0.4641196457903911</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>欲求周禮, 當得知周禮之人, 所謂是知周禮之人在於何處.在大水之一邊, 假喻以言遠.旣言此人在水一邊, 因以水行為喻.</t>
+          <t>鄭以為“蒹葭在衆草之中 蒼蒼然彊盛, 雖似不可雕傷, 至白露凝戾為霜, 則成而為黃矣, 以興衆民之彊者, 不從襄公敎令, 雖似不可屈服, 若得周禮以敎, 則衆民自然服矣. 欲求周禮, 當得知周禮之人, 所謂是知周禮之人在於何處. 在大水之一邊, 假喻以言遠. 旣言此人在水一邊, 因以水行為喻.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.4931362891058645</v>
+        <v>0.3634128328988683</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>若遡洄逆流而從之, 則道阻且長, 終不可見, 言不以敬順往求之, 則此人不可得之, 若遡游順流而從之, 則此人宛然在水中央, 易得見, 言以敬順求之, 則此人易得.何則?賢者, 難進而易退, 故不以敬順求之, 則不可得.欲令襄公敬順求知禮之賢人, 以敎其國也.”</t>
+          <t>若遡洄逆流而從之, 則道阻且長, 終不可見, 言不以敬順往求之, 則此人不可得之, 若遡游順流而從之, 則此人宛然在水中央, 易得見, 言以敬順求之, 則此人易得. 何則? 賢者, 難進而易退, 故不以敬順求之, 則不可得. 欲令襄公敬順求知禮之賢人, 以敎其國也.”</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1320,7 +1320,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.452242932702815</v>
+        <v>0.4651529505473779</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>傳‘蒹葭’至‘後興’ 正義曰：‘蒹 薕 葭 蘆’, 釋草文, 郭璞曰“蒹, 似萑而細, 高數尺.</t>
+          <t>傳‘蒹葭’至‘後興’ 正義曰：‘蒹 薕 葭 蘆’, 釋草文, 郭璞曰“蒹, 似萑而細, 高數尺. 蘆, 葦也.” 陸機疏云“蒹, 水草也, 堅實, 牛食之, 令牛肥彊. 靑․徐州人謂之蘆, 兗州․遼東通語也.” 祭義說養蠶之法云 “風戾以食之.” 注云 “使露氣燥乃食蠶.” 然則戾為燥之義. 下章‘未睎’, 謂露未乾(간)為霜. 然則露凝為霜, 亦如乾燥然, 故云‘凝戾為霜’, 探下章之意, 以為說也.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1348,7 +1348,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.8495117545044837</v>
+        <v>0.7449657287469301</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>蘆, 葦也.” 陸機疏云“蒹, 水草也, 堅實, 牛食之, 令牛肥彊.</t>
+          <t>傳‘蒹葭’至‘後興’ 正義曰：‘蒹 薕 葭 蘆’, 釋草文, 郭璞曰“蒹, 似萑而細, 高數尺. 蘆, 葦也.” 陸機疏云“蒹, 水草也, 堅實, 牛食之, 令牛肥彊. 靑․徐州人謂之蘆, 兗州․遼東通語也.” 祭義說養蠶之法云 “風戾以食之.” 注云 “使露氣燥乃食蠶.” 然則戾為燥之義. 下章‘未睎’, 謂露未乾(간)為霜. 然則露凝為霜, 亦如乾燥然, 故云‘凝戾為霜’, 探下章之意, 以為說也.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1376,7 +1376,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.5273107518321835</v>
+        <v>0.3923963077669553</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>靑․徐州人謂之蘆, 兗州․遼東通語也.”</t>
+          <t>傳‘蒹葭’至‘後興’ 正義曰：‘蒹 薕 葭 蘆’, 釋草文, 郭璞曰“蒹, 似萑而細, 高數尺. 蘆, 葦也.” 陸機疏云“蒹, 水草也, 堅實, 牛食之, 令牛肥彊. 靑․徐州人謂之蘆, 兗州․遼東通語也.” 祭義說養蠶之法云 “風戾以食之.” 注云 “使露氣燥乃食蠶.” 然則戾為燥之義. 下章‘未睎’, 謂露未乾(간)為霜. 然則露凝為霜, 亦如乾燥然, 故云‘凝戾為霜’, 探下章之意, 以為說也.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1404,7 +1404,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.7230416382779934</v>
+        <v>0.3530631429613892</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>祭義說養蠶之法云 “風戾以食之.”注云 “使露氣燥乃食蠶.”然則戾為燥之義.</t>
+          <t>傳‘蒹葭’至‘後興’ 正義曰：‘蒹 薕 葭 蘆’, 釋草文, 郭璞曰“蒹, 似萑而細, 高數尺. 蘆, 葦也.” 陸機疏云“蒹, 水草也, 堅實, 牛食之, 令牛肥彊. 靑․徐州人謂之蘆, 兗州․遼東通語也.” 祭義說養蠶之法云 “風戾以食之.” 注云 “使露氣燥乃食蠶.” 然則戾為燥之義. 下章‘未睎’, 謂露未乾(간)為霜. 然則露凝為霜, 亦如乾燥然, 故云‘凝戾為霜’, 探下章之意, 以為說也.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.3973419333116798</v>
+        <v>0.3467892891833441</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>下章‘未睎’, 謂露未乾(간)為霜.</t>
+          <t>傳‘蒹葭’至‘後興’ 正義曰：‘蒹 薕 葭 蘆’, 釋草文, 郭璞曰“蒹, 似萑而細, 高數尺. 蘆, 葦也.” 陸機疏云“蒹, 水草也, 堅實, 牛食之, 令牛肥彊. 靑․徐州人謂之蘆, 兗州․遼東通語也.” 祭義說養蠶之法云 “風戾以食之.” 注云 “使露氣燥乃食蠶.” 然則戾為燥之義. 下章‘未睎’, 謂露未乾(간)為霜. 然則露凝為霜, 亦如乾燥然, 故云‘凝戾為霜’, 探下章之意, 以為說也.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1460,7 +1460,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.4387528741984677</v>
+        <v>0.185150717774149</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>然則露凝為霜, 亦如乾燥然, 故云‘凝戾為霜’, 探下章之意, 以為說也.</t>
+          <t>傳‘蒹葭’至‘後興’ 正義曰：‘蒹 薕 葭 蘆’, 釋草文, 郭璞曰“蒹, 似萑而細, 高數尺. 蘆, 葦也.” 陸機疏云“蒹, 水草也, 堅實, 牛食之, 令牛肥彊. 靑․徐州人謂之蘆, 兗州․遼東通語也.” 祭義說養蠶之法云 “風戾以食之.” 注云 “使露氣燥乃食蠶.” 然則戾為燥之義. 下章‘未睎’, 謂露未乾(간)為霜. 然則露凝為霜, 亦如乾燥然, 故云‘凝戾為霜’, 探下章之意, 以為說也.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1488,7 +1488,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.73389977378655</v>
+        <v>0.3900605673430159</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>八月, 白露節, 秋分八月中, 九月, 寒露節, 霜降九月中. ‘白霜凝戾為霜然後歲事成’, 謂八月九月葭成葦, 可以為曲(簿)[薄]充歲事也.</t>
+          <t>八月, 白露節, 秋分八月中, 九月, 寒露節, 霜降九月中. ‘白霜凝戾為霜然後歲事成’, 謂八月九月葭成葦, 可以為曲(簿)[薄]充歲事也. 七月云 “八月萑葦”, 則八月葦已成. 此云‘白露為霜然後 歲事成’者, 以其霜降, 草乃成, 擧霜為言耳, 其實白露初降, 已任用矣. 此以霜降物成, 喻得禮則國興, 下章‘未晞’‘未已’, 言其未為霜則物不成, 喻未得禮則國不興. 此詩主刺未能用周禮, 故先言得禮則興, 後言無禮不興, 所以倒也.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1516,7 +1516,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.6475858553634266</v>
+        <v>0.5884012358819659</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>七月云 “八月萑葦”, 則八月葦已成.</t>
+          <t>八月, 白露節, 秋分八月中, 九月, 寒露節, 霜降九月中. ‘白霜凝戾為霜然後歲事成’, 謂八月九月葭成葦, 可以為曲(簿)[薄]充歲事也. 七月云 “八月萑葦”, 則八月葦已成. 此云‘白露為霜然後 歲事成’者, 以其霜降, 草乃成, 擧霜為言耳, 其實白露初降, 已任用矣. 此以霜降物成, 喻得禮則國興, 下章‘未晞’‘未已’, 言其未為霜則物不成, 喻未得禮則國不興. 此詩主刺未能用周禮, 故先言得禮則興, 後言無禮不興, 所以倒也.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1544,7 +1544,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.3452555731554267</v>
+        <v>0.5370104009060205</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>此云‘白露為霜然後 歲事成’者, 以其霜降, 草乃成, 擧霜為言耳, 其實白露初降, 已任用矣.</t>
+          <t>八月, 白露節, 秋分八月中, 九月, 寒露節, 霜降九月中. ‘白霜凝戾為霜然後歲事成’, 謂八月九月葭成葦, 可以為曲(簿)[薄]充歲事也. 七月云 “八月萑葦”, 則八月葦已成. 此云‘白露為霜然後 歲事成’者, 以其霜降, 草乃成, 擧霜為言耳, 其實白露初降, 已任用矣. 此以霜降物成, 喻得禮則國興, 下章‘未晞’‘未已’, 言其未為霜則物不成, 喻未得禮則國不興. 此詩主刺未能用周禮, 故先言得禮則興, 後言無禮不興, 所以倒也.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.2732342834439353</v>
+        <v>0.5068162120394476</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1591,16 +1591,16 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>此以霜降物成, 喻得禮則國興, 下章‘未晞’‘未已’, 言其未為霜則物不成, 喻未得禮則國不興.</t>
+          <t>八月, 白露節, 秋分八月中, 九月, 寒露節, 霜降九月中. ‘白霜凝戾為霜然後歲事成’, 謂八月九月葭成葦, 可以為曲(簿)[薄]充歲事也. 七月云 “八月萑葦”, 則八月葦已成. 此云‘白露為霜然後 歲事成’者, 以其霜降, 草乃成, 擧霜為言耳, 其實白露初降, 已任用矣. 此以霜降物成, 喻得禮則國興, 下章‘未晞’‘未已’, 言其未為霜則物不成, 喻未得禮則國不興. 此詩主刺未能用周禮, 故先言得禮則興, 後言無禮不興, 所以倒也.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>&lt;그런데&gt; 여기에서 ‘白露가 얼어 서리가 된 뒤에야 歲事가 이루어지고[白露為霜然後 歲事成]’라고 한 것은 서리가 내리는 때에야 풀이 마침내 다 자라므로 서리를 들어서 말한 것일 뿐이니 실제는 白露가 처음 내릴 때에도 이미 쓸 만하다.</t>
+          <t>&lt;그런데&gt; 여기에서 ‘白露가 얼어 서리가 된 뒤에야 歲事가 이루어지고[白露為 霜</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.304343910340669</v>
+        <v>0.4206059909907646</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1619,16 +1619,16 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>此詩主刺未能用周禮, 故先言得禮則興, 後言無禮不興, 所以倒也.</t>
+          <t>八月, 白露節, 秋分八月中, 九月, 寒露節, 霜降九月中. ‘白霜凝戾為霜然後歲事成’, 謂八月九月葭成葦, 可以為曲(簿)[薄]充歲事也. 七月云 “八月萑葦”, 則八月葦已成. 此云‘白露為霜然後 歲事成’者, 以其霜降, 草乃成, 擧霜為言耳, 其實白露初降, 已任用矣. 此以霜降物成, 喻得禮則國興, 下章‘未晞’‘未已’, 言其未為霜則物不成, 喻未得禮則國不興. 此詩主刺未能用周禮, 故先言得禮則興, 後言無禮不興, 所以倒也.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>여기는 서리가 내리면 갈대가 다 자라는 것으로 禮를 얻으면 나라가 흥성해짐을 비유한 것이고, 下章의 ‘未晞’와 ‘未已’는 &lt;白露가&gt; 서리가 되지 않으면 갈대가 다 자라지 않음을 말하여 禮를 얻지 못하면 나라가 흥성하지 못함을 비유한 것이다. 이 詩는 周禮를 잘 따르지 못함을 위주로 풍자한 것이다. 그리하여 禮를 얻으면 흥성함을 먼저 말하고 禮가 없으면 흥성하지 못함을 뒤에 말하였으니 이 때문에 뒤바뀐 것이다.</t>
+          <t>然後 歲事成]’라고 한 것은 서리가 내리는 때에야 풀이 마침내 다 자라므로 서리를 들어서 말한 것일 뿐이니 실제는 白露가 처음 내릴 때에도 이미 쓸 만하다.</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.4328039512682706</v>
+        <v>0.3948606831521131</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1637,26 +1637,26 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>箋‘蒹葭’至‘則服’ 正義曰：箋以序云‘未能用周禮 將無以固其國’, 當謂民未服從, 國未能固, 故易傳, 用周禮敎民, 則服.</t>
+          <t>八月, 白露節, 秋分八月中, 九月, 寒露節, 霜降九月中. ‘白霜凝戾為霜然後歲事成’, 謂八月九月葭成葦, 可以為曲(簿)[薄]充歲事也. 七月云 “八月萑葦”, 則八月葦已成. 此云‘白露為霜然後 歲事成’者, 以其霜降, 草乃成, 擧霜為言耳, 其實白露初降, 已任用矣. 此以霜降物成, 喻得禮則國興, 下章‘未晞’‘未已’, 言其未為霜則物不成, 喻未得禮則國不興. 此詩主刺未能用周禮, 故先言得禮則興, 後言無禮不興, 所以倒也.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>箋의 [蒹葭]에서 [則服]까지 正義曰：箋은 序에서 ‘周禮를 잘 따르지 못하여 그 나라를 견고하게 하지 못할 것이다. ’라고 한 것은 응당 백성이 복종하지 않아서 나라가 견고해지지 못함을 말한 것으로 여겼기 때문에 傳을 바꾸어 ‘周禮를 따라 백성을 교화하면 백성이 복종한다. ’고 한 것이다.</t>
+          <t>여기는 서리가 내리면 갈대가 다 자라는 것으로 禮를 얻으면 나라가 흥성해짐을 비유한 것이고, 下章의 ‘未晞’와 ‘未已’는 &lt;白露가&gt; 서리가 되지 않으면 갈대가 다 자라지 않음을 말하여 禮를 얻지 못하면 나라가 흥성하지 못함을 비유한 것이다. 이 詩는 周禮를 잘 따르지 못함을 위주로 풍자한 것이다. 그리하여 禮를 얻으면 흥성함을 먼저 말하고 禮가 없으면 흥성하지 못함을 뒤에 말하였으니 이 때문에 뒤바뀐 것이다.</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.7000018334404583</v>
+        <v>0.3702419360308905</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1665,26 +1665,26 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>傳‘伊維’至‘難至’ 正義曰：‘伊 維’, 釋詁文.傳以詩剌未能用周禮, 則未得人心, 則所謂維, 是得人之道也.</t>
+          <t>箋‘蒹葭’至‘則服’ 正義曰：箋以序云‘未能用周禮 將無以固其國’, 當謂民未服從, 國未能固, 故易傳, 用周禮敎民, 則服.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>傳의 [伊維]에서 [難至]까지 正義曰：‘伊 維’는 ≪爾雅≫ &lt;釋詁&gt;의 글이다.</t>
+          <t>箋의 [蒹葭]에서 [則服]까지 正義曰：箋은 序에서 ‘周禮를 잘 따르지 못하여 그 나라를 견고하게 하지 못할 것이다. ’라고 한 것은 응당 백성이 복종하지 않아서 나라가 견고해지지 못함을 말한 것으로 여겼기 때문에 傳을 바꾸어 ‘周禮를 따라 백성을 교화하면 백성이 복종한다. ’고 한 것이다.</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.7857675423019972</v>
+        <v>0.7000018334404583</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1703,16 +1703,16 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>下傳, 以遡洄喻逆禮, 遡游喻順禮, 言水內有得人之道, 在大水一方, 喻其遠而難至, 言得人之道 在禮樂之傍.</t>
+          <t>傳‘伊維’至‘難至’ 正義曰：‘伊 維’, 釋詁文. 傳以詩剌未能用周禮, 則未得人心, 則所謂維, 是得人之道也. 下傳, 以遡洄喻逆禮, 遡游喻順禮, 言水內有得人之道, 在大水一方, 喻其遠而難至, 言得人之道 在禮樂之傍.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>傳은 이 詩가 周禮를 따르지 못하면 인심을 얻지 못할 것임을 풍자한 것으로 여겼으니 그러고 보면 維라고 한 것은 &lt;주례대로 하는 것만이&gt; 사람을 얻는 방도여서이다.</t>
+          <t>傳의 [伊維]에서 [難至]까지 正義曰：‘伊 維’는 ≪爾雅≫ &lt;釋詁&gt;의 글이다.</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.4072767698610673</v>
+        <v>0.7385732532439735</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1731,16 +1731,16 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>須用禮樂以求之, 故下句言從水內以求所求之物, 喻用禮以求得人之道, 故王肅云 “維得人之道, 乃在水之一方.”</t>
+          <t>傳‘伊維’至‘難至’ 正義曰：‘伊 維’, 釋詁文. 傳以詩剌未能用周禮, 則未得人心, 則所謂維, 是得人之道也. 下傳, 以遡洄喻逆禮, 遡游喻順禮, 言水內有得人之道, 在大水一方, 喻其遠而難至, 言得人之道 在禮樂之傍.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>下傳은 ‘물살 거슬러 올라가는 것[遡洄]’으로 ‘예를 거스르는 것[逆禮]’을 비유하고 ‘물살 따라 가는 것[遡游]’으로 ‘예를 따르는 것[順禮]’을 비유하여 강물 안에 사람을 얻는 방도가 있음을 말한 것이고, ‘큰 강의 한편에 있다’는 것으로 멀리 있어 이르기 어려움을 비유하여 사람을 얻는 도가 禮樂 안에 있음을 말한 것이다. 반드시 예악으로 구하여야 하기 때문에 下句에서 물살 따라 강물 안에서 구하려는 대상을 구한다고 하여 禮를 따라 사람을 얻는 도를 구하는 것을 비유한 것이다. 그리하여 王肅이 “사람을 얻는 도는 강물 한편에 있다. ”라고 한 것이다.</t>
+          <t>傳은 이 詩가 周禮를 따르지 못하면 인심을 얻지 못할 것임을 풍자한 것으로 여겼으니 그러고 보면 維라고 한 것은 &lt;주례대로 하는 것만이&gt; 사람을 얻는 방도여서이다.</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.4463005132669446</v>
+        <v>0.5145551572080118</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1759,16 +1759,16 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>‘一方 難至矣’, 水以喻禮樂, 能用禮則至於道也.</t>
+          <t>傳‘伊維’至‘難至’ 正義曰：‘伊 維’, 釋詁文. 傳以詩剌未能用周禮, 則未得人心, 則所謂維, 是得人之道也. 下傳, 以遡洄喻逆禮, 遡游喻順禮, 言水內有得人之道, 在大水一方, 喻其遠而難至, 言得人之道 在禮樂之傍.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>‘一方 難至矣’는 물로 예악을 비유한 것이니 禮를 따르면 道에 이를 수 있는 것이다.</t>
+          <t>下傳은 ‘물살 거슬러 올라가는 것[遡洄]’으로 ‘예를 거스르는 것[逆禮]’을 비유하고 ‘물살 따라 가는 것[遡游</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.6821752760254132</v>
+        <v>0.476054272314103</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1777,26 +1777,26 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>箋‘伊當’至‘言遠’正義曰：箋以上句言用周禮敎民, 則民服, 此經當是勸君求賢人, 使之(周)[用]禮, 故易傳,</t>
+          <t>須用禮樂以求之, 故下句言從水內以求所求之物, 喻用禮以求得人之道, 故王肅云 “維得人之道, 乃在水之一方.” ‘一方 難至矣’, 水以喻禮樂, 能用禮則至於道也.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>箋의 [伊當]에서 [言遠]까지 正義曰：箋은 ‘上句에서 周禮를 따라 백성을 교화하면 백성들이 복종함을 말하였으니 여기의 經에서는 응당 군주에게 賢人을 찾아서 禮를 따르게 할 것을 권유한 것이다. ’라고 여겼다.</t>
+          <t>]’으로 ‘예를 따르는 것[順禮]’을 비유하여 강물 안에 사람을 얻는 방도가 있음을 말한 것이고, ‘큰 강의 한편에 있다’는 것으로 멀리 있어 이르기 어려움을 비유하여 사람을 얻는 도가 禮樂 안에 있음을 말한 것이다. 반드시 예악으로 구하여야 하기 때문에 下句에서 물살 따라 강물 안에서 구하려는 대상을 구한다고 하여 禮를 따라 사람을 얻는 도를 구하는 것을 비유한 것이다. 그리하여 王肅이 “사람을 얻는 도는 강물 한편에 있다. ”라고 한 것이다.</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.7026107043811464</v>
+        <v>0.4723510911850666</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1811,20 +1811,20 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>箋‘伊當’至‘言遠’正義曰：箋以上句言用周禮敎民, 則民服, 此經當是勸君求賢人, 使之(周)[用]禮, 故易傳,</t>
+          <t>須用禮樂以求之, 故下句言從水內以求所求之物, 喻用禮以求得人之道, 故王肅云 “維得人之道, 乃在水之一方.” ‘一方 難至矣’, 水以喻禮樂, 能用禮則至於道也.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>그리하여 傳을 바꾸어서 ‘이른바 그 분이[所謂伊人]’에 대하여 ‘이른바 이 周禮를 아는 賢人이 큰 강물 한편에 있다는 것이니 비유를 빌려 멀리 있음을 말한 것[所謂是知周禮之賢人 在大水一邊 假喻以言遠]’이라고 한 것이다.</t>
+          <t>‘一方 難至矣’는 물로 예악을 비유한 것이니 禮를 따르면 道에 이를 수 있는 것이다.</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.5387460970406219</v>
+        <v>0.5301323083434715</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1843,16 +1843,16 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>以所謂伊人, ‘所謂是知周禮之賢人 在大水一邊 假喻以言遠’, 故下句逆流․順流, 喻敬順, 皆述求賢之事.</t>
+          <t>箋‘伊當’至‘言遠’正義曰：箋以上句言用周禮敎民, 則民服, 此經當是勸君求賢人, 使之(周)[用]禮, 故易傳, 以所謂伊人,</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>그리하여 下句의 逆流와 順流도 공경과 순종을 비유한 것으로 모두 현자를 구하는 일을 서술한 것으로 여겼다.</t>
+          <t>箋의 [伊當]에서 [言遠]까지 正義曰：箋은 ‘上句에서 周禮를 따라 백성을 교화하면 백성들이 복종함을 말하였으니 여기의 經에서는 응당 군주에게 賢人을 찾아서 禮를 따르게 할 것을 권유한 것이다. ’라고 여겼다.</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.3863449255802231</v>
+        <v>0.6869152966819937</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1871,16 +1871,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>一邊, 水傍, 下云‘在湄’‘在涘’ 是其居水傍也.</t>
+          <t>箋‘伊當’至‘言遠’正義曰：箋以上句言用周禮敎民, 則民服, 此經當是勸君求賢人, 使之(周)[用]禮, 故易傳, 以所謂伊人,</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>一邊은 강가이니 아래에서 말한 ‘在湄’와 ‘在涘’는 강가에 있는 것이다.</t>
+          <t>그리하여 傳을 바꾸어서 ‘이른바 그 분이[所謂伊人]’에 대하여 ‘이른바 이 周禮를 아는 賢人이 큰 강물 한편에 있다는 것이니 비유를 빌려 멀리 있음을 말한 것[所謂是知周禮之賢人 在大水一邊 假喻以言遠]’이라고 한 것이다.</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.5931187393271997</v>
+        <v>0.5419217468355464</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1895,20 +1895,20 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>傳‘逆流’至‘以至’ 正義曰：</t>
+          <t>‘所謂是知周禮之賢人 在大水一邊 假喻以言遠’, 故下句逆流․順流, 喻敬順, 皆述求賢之事. 一邊, 水傍, 下云‘</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>傳의 [逆流]에서 [以至]까지 正義曰：≪爾雅≫ &lt;釋水&gt;에 “물살을 거슬러 올라가는 것을 ‘遡洄’라 하고 물살을 따라 내려가는 것을 ‘遡游’라 한다.</t>
+          <t>그리하여 下句의 逆流와 順流도 공경과 순종을 비유한 것으로 모두 현자를 구하는 일을 서술한 것으로 여겼다.</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.6968706130991233</v>
+        <v>0.3918155785038199</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1917,26 +1917,26 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>釋水云“逆流而上曰遡洄, 順流而下曰遡游.”</t>
+          <t>在湄’‘在涘’ 是其居水傍也.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>”라고 하였는데 孫炎은 “물살을 거슬러 건너는 것이 ‘逆流’이고 물살을 따라 건너는 것이 ‘順流’이다. ”라고 하였다.</t>
+          <t>一邊은 강가이니 아래에서 말한 ‘在湄’와 ‘在涘’는 강가에 있는 것이다.</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.3716873749985102</v>
+        <v>0.6352030922753459</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1955,16 +1955,16 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>孫炎曰 “逆渡者, 逆流也, 順渡者, 順流也.”</t>
+          <t>傳‘逆流’至‘以至’ 正義曰：釋水云“逆流而上曰遡洄, 順流而下曰遡游.” 孫炎曰 “逆渡者, 逆流也, 順渡者, 順流也.” 然則逆․順流, 皆謂渡水有逆順, 故下傳曰 ‘順流而涉’, 見(현)其是人渡水也. 此謂得人之道在於水邊, 逆流則道阻且長, 言其不可得至,</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>그렇다면 ‘逆流’와 ‘順流’는 모두 물을 건너는 방식에 물살을 거스르는 것과 따르는 것이 있음을 말한 것이다.</t>
+          <t>傳의 [逆流]에서 [以至]까지 正義曰：≪爾雅≫ &lt;釋水&gt;에 “물살을 거슬러 올라가는 것을 ‘遡洄’라 하고 물살을 따라 내려가는 것을 ‘遡游’라 한다.</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.5497107627955946</v>
+        <v>0.7100445521545666</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1973,7 +1973,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -1983,16 +1983,16 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>然則逆․順流, 皆謂渡水有逆順, 故下傳曰 ‘順流而涉’, 見(현)其是人渡水也. 此謂得人之道在於水邊, 逆流則道阻且長, 言其不可得至, 故喻逆禮則莫能以至, 言不得人之道, 不可至.</t>
+          <t>傳‘逆流’至‘以至’ 正義曰：釋水云“逆流而上曰遡洄, 順流而下曰遡游.” 孫炎曰 “逆渡者, 逆流也, 順渡者, 順流也.” 然則逆․順流, 皆謂渡水有逆順, 故下傳曰 ‘順流而涉’, 見(현)其是人渡水也. 此謂得人之道在於水邊, 逆流則道阻且長, 言其不可得至,</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>그리하여 下傳에 ‘물살 따라가며 건너는 것[順流而涉]’이라고 하였으니 바로 사람이 물을 건너는 것을 나타낸 것이다. 이 經文은 사람을 얻는 방도가 물가에 있거늘 흐름을 거슬러 가면 길이 험하고 멀다고 한 것이니 이를 수 없음을 말한 것이다. 그리하여 禮를 거스르면 이를 수 없음을 비유하여, 사람을 얻는 방도가 아니면 이를 수 없음을 말하였다.</t>
+          <t>”라고 하였는데 孫炎은 “물살을 거슬러 건너는 것이 ‘逆流’이고 물살을 따라 건너는 것이 ‘順流’이다. ”라고 하였다.</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.4954986887343831</v>
+        <v>0.4696117111978241</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -2011,16 +2011,16 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>上言得人之道 在水一方, 下句言水中央, 則是行未渡水, 禮自來水內, 故言順禮, 未濟, 道來迎之.</t>
+          <t>傳‘逆流’至‘以至’ 正義曰：釋水云“逆流而上曰遡洄, 順流而下曰遡游.” 孫炎曰 “逆渡者, 逆流也, 順渡者, 順流也.” 然則逆․順流, 皆謂渡水有逆順, 故下傳曰 ‘順流而涉’, 見(현)其是人渡水也. 此謂得人之道在於水邊, 逆流則道阻且長, 言其不可得至,</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>위에서는 사람을 얻는 방도가 강 한편에 있다고 말하였는데 下句에서는 강 가운데를 말한 것은, 물을 건너기 전에 禮가 있는 이가 스스로 강 가운데로 오기 때문에 예를 따르면 건너기 전에 道 있는 이가 와서 맞이한다고 한 것이다.</t>
+          <t>그렇다면 ‘逆流’와 ‘順流’는 모두 물을 건너는 방식에 물살을 거스르는 것과 따르는 것이 있음을 말한 것이다.</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.3861290155297268</v>
+        <v>0.546769423024965</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2029,7 +2029,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -2039,16 +2039,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>(未)[求]濟, 謂未渡水也, 以其用水為喻, 故以(未)[求]濟言之.</t>
+          <t>傳‘逆流’至‘以至’ 正義曰：釋水云“逆流而上曰遡洄, 順流而下曰遡游.” 孫炎曰 “逆渡者, 逆流也, 順渡者, 順流也.” 然則逆․順流, 皆謂渡水有逆順, 故下傳曰 ‘順流而涉’, 見(현)其是人渡水也. 此謂得人之道在於水邊, 逆流則道阻且長, 言其不可得至,</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>‘求濟’는 강을 건너기 전을 말하니 물로 비유를 삼았기 때문에 ‘求濟’라고 말한 것이다.</t>
+          <t>그리하여 下傳에 ‘물살 따라가며 건너는 것[順流而涉]’이라고 하였으니 바로 사람이 물을 건너는 것을 나타낸 것이다. 이 經文은 사람을 얻는 방도가 물가에 있거늘 흐름을 거슬러 가면 길이 험하고 멀다고 한 것이니 이를 수 없음을 말한 것이다. 그리하여 禮를 거스르면 이를 수 없음을 비유하여, 사람을 얻는 방도가 아니면 이를 수 없음을 말하였다.</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.4909418412332129</v>
+        <v>0.4745518431114496</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -2067,16 +2067,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>箋以伊人為知禮之人, 故易傳以為求賢之事.</t>
+          <t>故喻逆禮則莫能以至, 言不得人之道, 不可至. 上言得人之道 在水一方, 下句言水中央, 則是行未渡水, 禮自來水內, 故言順禮, 未濟, 道來迎之. (未)[求]濟, 謂未渡水也, 以其用水為喻, 故以(未)[求]濟言之. 箋以伊人為知禮之人, 故易傳以為求賢之事.</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>箋은 ‘伊人’을 禮를 아는 사람으로 여겼다. 그리하여 傳을 바꾸어 어진 이를 구하는 일로 여긴 것이다.</t>
+          <t>위에서는 사람을 얻는 방도가 강 한편에 있다고 말하였는데 下句에서는 강 가운데를 말한 것은, 물을 건너기 전에 禮가 있는 이가 스스로 강 가운데로 오기 때문에 예를 따르면 건너기 전에 道 있는 이가 와서 맞이한다고 한 것이다.</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0.7693160985102514</v>
+        <v>0.3689348527954708</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2085,26 +2085,26 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>蒹葭萋(처)萋하니 白露未晞로다</t>
+          <t>故喻逆禮則莫能以至, 言不得人之道, 不可至. 上言得人之道 在水一方, 下句言水中央, 則是行未渡水, 禮自來水內, 故言順禮, 未濟, 道來迎之. (未)[求]濟, 謂未渡水也, 以其用水為喻, 故以(未)[求]濟言之. 箋以伊人為知禮之人, 故易傳以為求賢之事.</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>갈대 무성하니 白露 아직 마르지 않았네</t>
+          <t>‘求濟’는 강을 건너기 전을 말하니 물로 비유를 삼았기 때문에 ‘求濟’라고 말한 것이다.</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.4004411587478217</v>
+        <v>0.3615212762431278</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2113,26 +2113,26 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>萋萋는 猶蒼蒼也라 晞는 乾(간)也라</t>
+          <t>故喻逆禮則莫能以至, 言不得人之道, 不可至. 上言得人之道 在水一方, 下句言水中央, 則是行未渡水, 禮自來水內, 故言順禮, 未濟, 道來迎之. (未)[求]濟, 謂未渡水也, 以其用水為喻, 故以(未)[求]濟言之. 箋以伊人為知禮之人, 故易傳以為求賢之事.</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>‘萋萋’는 ‘蒼蒼’과 같다. 晞는 ‘마르다’이다.</t>
+          <t>箋은 ‘伊人’을 禮를 아는 사람으로 여겼다. 그리하여 傳을 바꾸어 어진 이를 구하는 일로 여긴 것이다.</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.6883855017940126</v>
+        <v>0.3976936511515896</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2141,26 +2141,26 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>箋云 未晞는 未為霜이라</t>
+          <t>蒹葭萋(처)萋하니 白露未晞로다</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>箋云：‘未晞’는 아직 서리가 되지 않은 것이다.</t>
+          <t>갈대 무성하니 白露 아직 마르지 않았네</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.719907211279909</v>
+        <v>0.4004411587478217</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2175,20 +2175,20 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>傳‘晞 乾’ 正義曰：湛露云“匪陽不晞”, 言見日則乾, 故知晞為乾也.</t>
+          <t>萋萋는 猶蒼蒼也라 晞는 乾(간)也라</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>傳의 [晞 乾] 正義曰：&lt;小雅 湛露&gt;에 “햇볕이 아니면 마르지 않네[匪陽不晞]”라고 하였으니 햇볕을 쬐면 마르는 것을 말한 것이다. 그리하여 晞가 ‘마르다’임을 안 것이다.</t>
+          <t>‘萋萋’는 ‘蒼蒼’과 같다. 晞는 ‘마르다’이다.</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0.6346660768449383</v>
+        <v>0.6883855017940126</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2203,20 +2203,20 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>彼言露晞, 謂露盡乾.</t>
+          <t>箋云 未晞는 未為霜이라</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>&lt;湛露&gt;에서 ‘露晞’라고 한 것은 이슬이 다 마른 것을 말한다.</t>
+          <t>箋云：‘未晞’는 아직 서리가 되지 않은 것이다.</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.5776927038217512</v>
+        <v>0.719907211279909</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2235,16 +2235,16 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>此篇上章言白露為霜, 則此言未晞, 謂未乾為霜,</t>
+          <t>傳‘晞 乾’ 正義曰：湛露云“匪陽不晞”, 言見日則乾, 故知晞為乾也. 彼言露晞, 謂露盡乾.</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>그런데 이 시의 上章에서 ‘白露 서리가 되었네[白露為霜]’라고 하였으니 이 章에서 말한 ‘未晞’는 말라서 서리가 되지 않은 것을 말하니 &lt;湛露&gt;와는 &lt;晞의 의미가&gt; 다르다.</t>
+          <t>傳의 [晞 乾] 正義曰：&lt;小雅 湛露&gt;에 “햇볕이 아니면 마르지 않네[匪陽不晞]”라고 하였으니 햇볕을 쬐면 마르는 것을 말한 것이다. 그리하여 晞가 ‘마르다’임을 안 것이다.</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0.6951338124968726</v>
+        <v>0.622220784618351</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
@@ -2263,16 +2263,16 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>與彼異, 故箋云 ‘未晞 未為霜也’.</t>
+          <t>傳‘晞 乾’ 正義曰：湛露云“匪陽不晞”, 言見日則乾, 故知晞為乾也. 彼言露晞, 謂露盡乾.</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>그리하여 箋에서 ‘未晞는 서리가 되지 않은 것이다.[未晞 未為霜也]’라고 한 것이다.</t>
+          <t>&lt;湛露&gt;에서 ‘露晞’라고 한 것은 이슬이 다 마른 것을 말한다.</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0.6057961860165383</v>
+        <v>0.5358801528724824</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2281,26 +2281,26 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>所謂伊人이 在水之湄언마는</t>
+          <t>此篇上章言白露為霜, 則此言未晞, 謂未乾為霜, 與彼異, 故箋云 ‘未晞 未為霜也’.</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>이른바 그분이 강물 가에 있건만</t>
+          <t>그런데 이 시의 上章에서 ‘白露 서리가 되었네[白露為霜]’라고 하였으니 이 章에서 말한 ‘未晞’는 말라서 서리가 되지 않은 것을 말하니 &lt;湛露&gt;와는 &lt;晞의 의미가&gt; 다르다. 그리하여 箋에서 ‘未晞는 서리가 되지 않은 것이다.</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.2469248040159258</v>
+        <v>0.7028170404547954</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2309,26 +2309,26 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>湄는 水隒(엄)이라</t>
+          <t>此篇上章言白露為霜, 則此言未晞, 謂未乾為霜, 與彼異, 故箋云 ‘未晞 未為霜也’.</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>湄는 ‘물가’이다.</t>
+          <t>[未晞 未為霜也]’라고 한 것이다.</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.664997316046769</v>
+        <v>0.6728995748300934</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2337,26 +2337,26 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>傳‘湄 水隒’正義曰 ; 釋水云“水草交為湄.”謂水草交際之處, 水之岸也.釋山云</t>
+          <t>所謂伊人이 在水之湄언마는</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>傳의 [湄 水隒] 正義曰：≪爾雅≫ &lt;釋水&gt;에 “강물이 풀에 닿는 곳이 湄이다. ”라고 하였으니 물과 풀이 만나는 곳을 말하니 강기슭이다.</t>
+          <t>이른바 그분이 강물 가에 있건만</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.6773385162164326</v>
+        <v>0.2469248040159258</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2371,20 +2371,20 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>“重甗(언), 隒(엄).” 隒, 是山岸, 湄, 是水岸, 故云‘水隒.’</t>
+          <t>湄는 水隒(엄)이라</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>≪爾雅≫ &lt;釋山&gt;에 “두 개의 시루가 포개진 것과 같은 곳이 隒이다. ”라고 하였으니 隒은 산기슭이고 湄는 강기슭이다. 그리하여 ‘水隒’이라고 한 것이다.</t>
+          <t>湄는 ‘물가’이다.</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.5414792118482668</v>
+        <v>0.664997316046769</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2399,20 +2399,20 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>遡洄從之하니 道阻且躋러니</t>
+          <t>傳‘湄 水隒’正義曰 ; 釋水云“水草交為湄.” 謂水草交際之處, 水之岸也.</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>거슬러 올라가 따르려하니 길은 험하고 오르막이더니</t>
+          <t>傳의 [湄 水隒] 正義曰：≪爾雅≫ &lt;釋水&gt;에 “강물이 풀에 닿는 곳이 湄이다. ”라고 하였으니 물과 풀이 만나는 곳을 말하니 강기슭이다.</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.3162463393532332</v>
+        <v>0.6946975593756352</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2427,20 +2427,20 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>躋는 升也라</t>
+          <t>釋山云 “重甗(언), 隒(엄).” 隒, 是山岸, 湄, 是水岸, 故云‘水隒.’</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>躋는 ‘오르막’이다.</t>
+          <t>≪爾雅≫ &lt;釋山&gt;에 “두 개의 시루가 포개진 것과 같은 곳이 隒이다. ”라고 하였으니 隒은 산기슭이고 湄는 강기슭이다. 그리하여 ‘水隒’이라고 한 것이다.</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.4882438233054427</v>
+        <v>0.5275218839229604</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2455,20 +2455,20 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>箋云：升者는 言其難至니 如升阪이라 躋는 本又作隮라</t>
+          <t>遡洄從之하니 道阻且躋러니</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>升은 이르기 어려움을 말하니 비탈을 오르는 것과 같은 것이다. 躋는 隮로 되어 있는 본도 있다.</t>
+          <t>거슬러 올라가 따르려하니 길은 험하고 오르막이더니</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.47923560286808</v>
+        <v>0.3162463393532332</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2483,20 +2483,20 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>遡游從之하니 宛在水中坻(지)로다</t>
+          <t>躋는 升也라</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>물살 따라 가니 가만히 강 가운데 모래톱에 있다네</t>
+          <t>躋는 ‘오르막’이다.</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.3063424195635974</v>
+        <v>0.4882438233054427</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2511,20 +2511,20 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>坻는 小渚也라</t>
+          <t>箋云：升者는 言其難至니 如升阪이라 躋는 本又作隮라</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>坻는 작은 모래톱이다.</t>
+          <t>升은 이르기 어려움을 말하니 비탈을 오르는 것과 같은 것이다. 躋는 隮로 되어 있는 본도 있다.</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0.5662669337905479</v>
+        <v>0.47923560286808</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2539,20 +2539,20 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>傳‘坻 小渚’正義曰：釋水云“小洲曰渚, 小渚曰沚, 小沚曰坻.”</t>
+          <t>遡游從之하니 宛在水中坻(지)로다</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>傳의 [坻小渚] 正義曰：≪爾雅≫ &lt;釋水&gt;에 “洲보다 작은 모래톱[小洲]을 渚라 하고, 渚보다 작은 모래톱[小渚]을 沚라 하고, 沚보다 작은 모래톱[小沚]을 坻라고 한다. ”라고 하였다.</t>
+          <t>물살 따라 가니 가만히 강 가운데 모래톱에 있다 네</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.6987789752870318</v>
+        <v>0.2976789429690118</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2567,20 +2567,20 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>然則坻, 是小沚, 言小渚者, 渚․沚 皆水中之地, 小大異也.以渚易知, 故繫渚言之.</t>
+          <t>坻는 小渚也라</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>그렇다면 坻는 ‘小沚’인데 &lt;傳에서&gt; ‘小渚’라고 한 것은, 渚나 沚가 모두 물 가운데 있는 땅으로 그 크기가 다른데 ‘渚’가 알기 쉽기 때문에  渚를 붙여 말한 것이다.</t>
+          <t>坻는 작은 모래톱이다.</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.7183243138768276</v>
+        <v>0.5662669337905479</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2595,20 +2595,20 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>蒹葭采采하니 白露未已로다</t>
+          <t>傳‘坻 小渚’正義曰：釋水云“小洲曰渚, 小渚曰沚, 小沚曰坻.” 然則坻,</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>갈대 무성하니 白露 아직 그치지 않았네</t>
+          <t>傳의 [坻小渚] 正義曰：≪爾雅≫ &lt;釋水&gt;에 “洲보다 작은 모래톱[小洲]을 渚라 하고, 渚보다 작은 모래톱[小渚]을 沚라 하고, 沚보다 작은 모래톱[小沚]을 坻라고 한다. ”라고 하였다.</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.4355140612433351</v>
+        <v>0.6656959302026643</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2623,20 +2623,20 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>采采는 猶萋萋也라 未已는 猶未止也라</t>
+          <t>是小沚, 言小渚者, 渚․沚 皆水中之地, 小大異也. 以渚易知, 故繫渚言之.</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>‘采采’는 ‘萋萋’와 같다.</t>
+          <t>그렇다면 坻는 ‘小沚’인데 &lt;傳에서&gt; ‘小渚’라고 한 것은, 渚나 沚가 모두 물 가운데 있는 땅으로 그 크기가 다른데 ‘渚’가 알기 쉽기 때문에  渚를 붙여 말한 것이다.</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.6577254270485263</v>
+        <v>0.7470665523128781</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2645,26 +2645,26 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>target_rich</t>
+          <t>sequential_1to1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>采采는 猶萋萋也라 未已는 猶未止也라</t>
+          <t>蒹葭采采하니 白露未已로다</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>‘未已’는 ‘未止’와 같다.</t>
+          <t>갈대 무성하니 白露 아직 그치지 않았네</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.4976758773912755</v>
+        <v>0.4355140612433351</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2673,26 +2673,26 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>target_rich</t>
+          <t>sequential_1to1</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>所謂伊人이 在水之涘(사)언마는</t>
+          <t>采采는 猶萋萋也라 未已는 猶未止也라</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>이른바 그 분이 강가에 있건만</t>
+          <t>‘采采’는 ‘萋萋’와 같다.</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.2812653299563516</v>
+        <v>0.6577254270485263</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2701,26 +2701,26 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>涘는 厓也라</t>
+          <t>采采는 猶萋萋也라 未已는 猶未止也라</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>涘는 ‘강가’이다.</t>
+          <t>‘未已’는 ‘未止’와 같다.</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0.5306944118124213</v>
+        <v>0.4976758773912755</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2729,26 +2729,26 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>sequential_1to1</t>
+          <t>target_rich</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>遡洄從之하니 道阻且右러니</t>
+          <t>所謂伊人이 在水之涘(사)언마는</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>물살 거슬러 따라가니 길이 험하고 우회하더니</t>
+          <t>이른바 그 분이 강가에 있건만</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0.355588050928784</v>
+        <v>0.2812653299563516</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2763,20 +2763,20 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>右는 出其右也라</t>
+          <t>涘는 厓也라</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>右는 우측으로 돌아서 나가는 것이다.</t>
+          <t>涘는 ‘강가’이다.</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0.3859058123387094</v>
+        <v>0.5306944118124213</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2791,20 +2791,20 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>箋云 右者는 言其迂迴也라</t>
+          <t>遡洄從之하니 道阻且右러니</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>箋云：右는 우회함을 말한 것이다.</t>
+          <t>물살 거슬러 따라가니 길이 험하고 우회하더니</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0.6081469188059594</v>
+        <v>0.355588050928784</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2819,20 +2819,20 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>傳‘右 出其右’ 正義曰：此說道路艱難, 而云‘且右’, 故知右謂出其右也.若正與相當, 行則易到, 今乃出其右廂, 是難至也.</t>
+          <t>右는 出其右也라</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>傳의 [右 出其右] 正義曰：이는 길이 험난함을 말하면서 ‘且右’라고 하였기 때문에 右가 우측으로 돌아 나가는 것임을 안 것이다. 만약 물살 흐르는 대로 따라가면 쉽게 이르는데 지금 오히려 우측으로 돌아 나가니 이는 이르기 어려운 것이다. 箋에 ‘右는 우회함을 말한 것이다. ’라고 하였는데, 좌측으로 돌아 나가는 것도 역시 우회하는 것이다.</t>
+          <t>右는 우측으로 돌아서 나가는 것이다.</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0.6607568658931418</v>
+        <v>0.3859058123387094</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2847,20 +2847,20 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>箋云 ‘右 言其迂迴’, 出其左, 亦迂迴, 言右, 取其與涘․沚為韻.</t>
+          <t>箋云 右者는 言其迂迴也라</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>그런데 右라고 한 것은 涘․沚와 韻을 맞추기 위한 것이다.</t>
+          <t>箋云：右는 우회함을 말한 것이다.</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0.5293871379887644</v>
+        <v>0.6081469188059594</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2875,20 +2875,20 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>遡游從之하니 宛在水中沚로다</t>
+          <t>傳‘右 出其右’ 正義曰：此說道路艱難, 而云‘且右’, 故知右謂出其右也. 若正與相當, 行則易到, 今乃出其右廂, 是難至也.</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>물살 따라 가니 가만히 물 가운데 작은 모래톱에 있네</t>
+          <t>傳의 [右 出其右] 正義曰：이는 길이 험난함을 말하면서 ‘且右’라고 하였기 때문에 右가 우측으로 돌아 나가는 것임을 안 것이다. 만약 물살 흐르는 대로 따라가면 쉽게 이르는데 지금 오히려 우측으로 돌아 나가니 이는 이르기 어려운 것이다. 箋에 ‘右는 우회함을 말한 것이다. ’라고 하였는데, 좌측으로 돌아 나가는 것도 역시 우회하는 것이다.</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>0.3419277899033674</v>
+        <v>0.6617175017434926</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2903,20 +2903,20 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>小渚曰沚라</t>
+          <t>箋云 ‘右 言其迂迴’, 出其左, 亦迂迴, 言右, 取其與涘․沚為韻.</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>작은 모래톱을 沚라고 한다.</t>
+          <t>그런데 右라고 한 것은 涘․沚와 韻을 맞추기 위한 것이다.</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>0.5092054802469561</v>
+        <v>0.5293871379887644</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2931,27 +2931,83 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
+        <v>44</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>遡游從之하니 宛在水中沚로다</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>물살 따라 가니 가만히 물 가운데 작은 모래톱에 있네</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.3419277899033674</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>spacy_lg</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>sequential_1to1</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>45</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>小渚曰沚라</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>작은 모래톱을 沚라고 한다.</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.5092054802469561</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>spacy_lg</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>sequential_1to1</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
         <v>46</v>
       </c>
-      <c r="B90" t="inlineStr">
+      <c r="B92" t="inlineStr">
         <is>
           <t>蒹葭 三章이니 章八句라</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
+      <c r="C92" t="inlineStr">
         <is>
           <t>&lt;蒹葭&gt; 3章이니 章마다 8句이다.</t>
         </is>
       </c>
-      <c r="D90" t="n">
+      <c r="D92" t="n">
         <v>0.8031119812229623</v>
       </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>spacy_lg</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>spacy_lg</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
         <is>
           <t>sequential_1to1</t>
         </is>

</xml_diff>